<commit_message>
Updated file structure and second issue added
</commit_message>
<xml_diff>
--- a/Equations/00_nomenclature_definition.xlsx
+++ b/Equations/00_nomenclature_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0093836\Box Sync\My Webspace\Post-doc\Spine\WP3\Equations\equations_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0093836\Box Sync\My Webspace\Post-doc\Spine\WP3\model\Equations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1487,9 +1487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>